<commit_message>
more fixes part 5
</commit_message>
<xml_diff>
--- a/inst/extdata/Example_MHQuant_Small_metadata_tables.xlsx
+++ b/inst/extdata/Example_MHQuant_Small_metadata_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/tests/testthat/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3414D5C1-384C-BF4A-AD8E-EFBB03DD5DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0AD108-2E95-0F45-B069-DC9112FB2283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
@@ -1091,13 +1091,13 @@
       <sheetName val="Features (Analytes)"/>
       <sheetName val="Internal Standards"/>
       <sheetName val="Response Curves"/>
-      <sheetName val="Calibration Curves"/>
+      <sheetName val="QC Concentrations"/>
       <sheetName val="Instructions"/>
       <sheetName val="About"/>
       <sheetName val="Lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
@@ -1429,13 +1429,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1A2D03-4C83-7448-999B-AC6C8C01C8BE}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -3723,7 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEF20C9-E726-8549-8B20-6F3F3BE0DDC1}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>